<commit_message>
Added RAM Mount Costs
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -183,9 +183,6 @@
     <t xml:space="preserve">Appx Shipping + Tax </t>
   </si>
   <si>
-    <t>Misc (Jumpers, heat shrink, etc.)</t>
-  </si>
-  <si>
     <t>Actual Total</t>
   </si>
   <si>
@@ -205,6 +202,21 @@
   </si>
   <si>
     <t>Posi-Lock</t>
+  </si>
+  <si>
+    <t>RAM Mount Steel U-Bolt Rail Base with Short Arm Diamond Assembly</t>
+  </si>
+  <si>
+    <t>RAM Mount Hardware for Cradles</t>
+  </si>
+  <si>
+    <t>SKU:RAMSHOL</t>
+  </si>
+  <si>
+    <t>SKU:RAMB149-A</t>
+  </si>
+  <si>
+    <t>GPSCity</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +274,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -321,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,6 +379,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,15 +685,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.85546875" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
@@ -1256,10 +1285,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="D27" s="21">
         <v>1</v>
@@ -1277,10 +1306,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" s="21">
         <v>1</v>
@@ -1298,10 +1327,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="D29" s="6">
         <v>3</v>
@@ -1324,7 +1353,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>4</v>
@@ -1337,30 +1366,77 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="A32" s="7">
+        <v>28</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="25">
+        <v>1</v>
+      </c>
+      <c r="E32" s="26">
+        <v>27.95</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" ref="F32:F33" si="11">D32*E32</f>
+        <v>27.95</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>29</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="25">
+        <v>1</v>
+      </c>
+      <c r="E33" s="26">
+        <v>2.8</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="11"/>
+        <v>2.8</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="F34" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19">
-        <f>SUM(F32:F33)+F31</f>
-        <v>140.32000000000002</v>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="19">
+        <f>SUM(F32:F35)+F31</f>
+        <v>171.07000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated components for V2
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="11475" windowHeight="5445" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -233,12 +233,6 @@
     <t>http://www.sparkfun.com/products/11113</t>
   </si>
   <si>
-    <t>http://www.sparkfun.com/products/9716</t>
-  </si>
-  <si>
-    <t>FTDI Basic Breakout - 5V</t>
-  </si>
-  <si>
     <t>LM2940 5V REGULATOR</t>
   </si>
   <si>
@@ -251,28 +245,103 @@
     <t>http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6#ht_2092wt_1163</t>
   </si>
   <si>
-    <t>Radio Shack</t>
-  </si>
-  <si>
-    <t>Mini through board</t>
-  </si>
-  <si>
-    <t>Battery Voltage Div Resistor 1 - MilSpec</t>
-  </si>
-  <si>
-    <t>Battery Voltage Div Resistor 2 - MilSpec</t>
-  </si>
-  <si>
-    <t>Gear Voltage Div Resistors - MilSpec</t>
-  </si>
-  <si>
     <t>I2C LCD Display (16x2)</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d#ht_3637wt_1163</t>
   </si>
   <si>
-    <t>Screws</t>
+    <t>Schematic Name</t>
+  </si>
+  <si>
+    <t>Din</t>
+  </si>
+  <si>
+    <t>Nano1</t>
+  </si>
+  <si>
+    <t>Rin</t>
+  </si>
+  <si>
+    <t>LM2940</t>
+  </si>
+  <si>
+    <t>Cin1</t>
+  </si>
+  <si>
+    <t>Cin2</t>
+  </si>
+  <si>
+    <t>Cout</t>
+  </si>
+  <si>
+    <t>Led6</t>
+  </si>
+  <si>
+    <t>Led1</t>
+  </si>
+  <si>
+    <t>Led2, Led3</t>
+  </si>
+  <si>
+    <t>Led4, Led5</t>
+  </si>
+  <si>
+    <t>Cds</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>Rcds</t>
+  </si>
+  <si>
+    <t>Rgps1, Rgps2</t>
+  </si>
+  <si>
+    <t>Rbatt1</t>
+  </si>
+  <si>
+    <t>Rbatt2</t>
+  </si>
+  <si>
+    <t>Rled1 .. Rled6</t>
+  </si>
+  <si>
+    <t>http://www.radioshack.com/product/index.jsp?productId=2102845</t>
+  </si>
+  <si>
+    <t>Radio shack PCB 417 Holes</t>
+  </si>
+  <si>
+    <t>Model: 276-150  | Catalog #: 276-150</t>
+  </si>
+  <si>
+    <t>DIGIKEY: CMF499KHBCT-ND</t>
+  </si>
+  <si>
+    <t>Gear Voltage Div Resistors - MilSpec - 499KOhm</t>
+  </si>
+  <si>
+    <t>DIGIKEY: CMF953KHBCT-ND</t>
+  </si>
+  <si>
+    <t>DIGIKEY: CMF332KHBCT-ND</t>
+  </si>
+  <si>
+    <t>Battery Voltage Div Resistor 2 - MilSpec - 953KOhm</t>
+  </si>
+  <si>
+    <t>Battery Voltage Div Resistor 1 - MilSpec - 332KOhm</t>
+  </si>
+  <si>
+    <t>PhotoCell Voltage Divider Resistor - 10KOhm, 1/8W</t>
+  </si>
+  <si>
+    <t>EBAY</t>
+  </si>
+  <si>
+    <t>*Generic</t>
   </si>
 </sst>
 </file>
@@ -349,11 +418,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -410,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -445,9 +513,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B34" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,23 +1603,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1560,12 +1628,13 @@
       <c r="C1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1573,671 +1642,674 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
         <v>18.95</v>
       </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
+      <c r="G3" s="8">
+        <f>E3*F3</f>
         <v>18.95</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7">
-        <v>15</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" ref="F4:F28" si="0">D4*E4</f>
-        <v>15</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>72</v>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.32</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G25" si="0">E4*F4</f>
+        <v>0.32</v>
       </c>
       <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0.32</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="0"/>
-        <v>0.32</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
         <v>0.59</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1.89</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" ref="G6" si="1">E6*F6</f>
+        <v>1.89</v>
+      </c>
       <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>4</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1.89</v>
-      </c>
-      <c r="F7" s="8">
-        <f t="shared" si="0"/>
-        <v>1.89</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="G7" s="8">
+        <f>E7*F7</f>
+        <v>0.45</v>
+      </c>
       <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>4</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1.89</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" ref="F8" si="1">D8*E8</f>
-        <v>1.89</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
         <v>0.45</v>
       </c>
-      <c r="F9" s="8">
-        <f>D9*E9</f>
-        <v>0.45</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.45</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C9" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
         <v>0.31</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="G10" s="8">
+        <f>E10*F10</f>
+        <v>0.23</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="8">
+        <f>E11*F11</f>
+        <v>0.8</v>
+      </c>
       <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0.18</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>9</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="F13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.23</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="10">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8">
         <v>0.53</v>
       </c>
-      <c r="F14" s="8">
+      <c r="G12" s="8">
         <f t="shared" si="0"/>
         <v>1.06</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="10">
-        <v>2</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="F15" s="8">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="B13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.18</v>
+      </c>
+      <c r="G13" s="8">
+        <f>E13*F13</f>
+        <v>0.18</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
         <v>1.86</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G14" s="8">
         <f t="shared" si="0"/>
         <v>1.86</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="8">
+        <f>E15*F15</f>
+        <v>0.15</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <f>E16*F16</f>
+        <v>2</v>
+      </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="10">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
+        <v>40</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="10">
+        <v>6</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="8">
+        <f>E17*F17</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" ref="G18:G19" si="2">E18*F18</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8">
         <v>12</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G20" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>14</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="H20" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
         <v>1.6</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G21" s="8">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>15</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="H21" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G22" s="8">
+        <f>E22*F22</f>
+        <v>0.3</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="10">
-        <v>1</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
         <v>6.52</v>
       </c>
-      <c r="F19" s="8">
+      <c r="G23" s="8">
         <f t="shared" si="0"/>
         <v>6.52</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>16</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
-        <v>2</v>
-      </c>
-      <c r="F20" s="8">
-        <v>2</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="10">
-        <v>6</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F21" s="8">
-        <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>20</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="12">
-        <v>2</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F22" s="8">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>21</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="12">
-        <v>1</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F23" s="8">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="12">
-        <v>1</v>
-      </c>
-      <c r="E24" s="8">
-        <v>1</v>
+      <c r="B24" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="19">
+        <v>3</v>
       </c>
       <c r="F24" s="8">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="12">
-        <v>1</v>
-      </c>
-      <c r="E25" s="8">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="B25" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="G25" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>24</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="12">
-        <v>2</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>27</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="19">
-        <v>3</v>
-      </c>
-      <c r="E27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>28</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>4</v>
-      </c>
-      <c r="F28" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4">
-        <f>SUM(F3:F28)</f>
-        <v>78.450000000000017</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="22"/>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="18" t="s">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="H25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="4">
+        <f>SUM(G3:G25)</f>
+        <v>58.04999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="22"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="17">
-        <f>SUM(F30:F33)+F29</f>
-        <v>78.450000000000017</v>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="17">
+        <f>SUM(G27:G30)+G26</f>
+        <v>58.04999999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G27" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="H18" r:id="rId4" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
-    <hyperlink ref="H17" r:id="rId5" location="ht_3637wt_1163" display="http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d - ht_3637wt_1163"/>
+    <hyperlink ref="H24" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H21" r:id="rId3" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
+    <hyperlink ref="H20" r:id="rId4" location="ht_3637wt_1163" display="http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d - ht_3637wt_1163"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated: Added posi-tap and more descriptions
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11475" windowHeight="5445" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="11475" windowHeight="5385"/>
   </bookViews>
   <sheets>
-    <sheet name="Gen1" sheetId="1" r:id="rId1"/>
-    <sheet name="Gen2" sheetId="2" r:id="rId2"/>
+    <sheet name="Gen2" sheetId="2" r:id="rId1"/>
+    <sheet name="Gen1 (OBSOLETE)" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -345,6 +345,126 @@
   </si>
   <si>
     <t>Arduino Nano V3 (or compatible)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERG-3SJ160/P16W-3BK-ND/36658</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=LM2940T-5.0-ND&amp;x=21&amp;y=17&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?vendor=0&amp;keywords=P5541-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=445-2870-ND&amp;x=20&amp;y=15&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=P12927-ND&amp;x=21&amp;y=21&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>Temp Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MeasureBattery </t>
+  </si>
+  <si>
+    <t>Photo Cell</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/C503B-GCN-CY0C0791/C503B-GCN-CY0C0791-ND/1922940</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en/optoelectronics/leds-discrete/524729?k=67-1117-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=C503B-WAN-CCACB151-ND&amp;x=11&amp;y=13&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/C503B-BCS-CV0Z0461/C503B-BCS-CV0Z0461-ND/1922944</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CMF55499K00BEEB/CMF499KHBCT-ND/2197183</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CMF55332K00BEEB/CMF332KHBCT-ND/2197180</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CMF55953K00BEEB/CMF953KHBCT-ND/2197185</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=PDV-P8001-ND&amp;x=17&amp;y=15&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=HM1038-ND&amp;x=15&amp;y=14&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Measures ambient light to control brightness of backlit LCD display and LEDs</t>
+  </si>
+  <si>
+    <t>Circuit board to connect everything together.</t>
+  </si>
+  <si>
+    <t>Brain - Microcontroller</t>
+  </si>
+  <si>
+    <t>Part of 12V-&gt;5V power regulator</t>
+  </si>
+  <si>
+    <t>Gear Position indicator</t>
+  </si>
+  <si>
+    <t>Limit current of Gear Position indicator LEDs</t>
+  </si>
+  <si>
+    <t>Main Display</t>
+  </si>
+  <si>
+    <t>Digital Temperature Sensor</t>
+  </si>
+  <si>
+    <t>Enclosure (Box) to hold all components</t>
+  </si>
+  <si>
+    <t>Part of gear  voltage meter circuit</t>
+  </si>
+  <si>
+    <t>Part of PhotoCell circuit</t>
+  </si>
+  <si>
+    <t>Part of battery voltage meter circuit</t>
+  </si>
+  <si>
+    <t>Part of digital temperature sensor circuit</t>
+  </si>
+  <si>
+    <t>Optional - used to connect/disconnect wires quickly without soldering</t>
+  </si>
+  <si>
+    <t>Posi-Tap - 16-18 AWG (BLUE)</t>
+  </si>
+  <si>
+    <t>Posi-Tap</t>
+  </si>
+  <si>
+    <t>Optional - used to tap into the V-Strom  GPS (the pink wire)</t>
+  </si>
+  <si>
+    <t>Note that these are only necessary if you want to color code your gears.  If you want to have the same color for all gears then get all the same color LEDs.</t>
+  </si>
+  <si>
+    <t>http://www.posi-lock.com/posiplug.html</t>
+  </si>
+  <si>
+    <t>Note that posi-lock products come in packages. Try to find cheaper single distributions, or buy with other stromtroopers are share the cost</t>
   </si>
 </sst>
 </file>
@@ -355,7 +475,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,8 +546,15 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +576,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,7 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -518,6 +657,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -820,6 +979,898 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*G3</f>
+        <v>10</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" ref="H4:H25" si="0">F4*G4</f>
+        <v>0.59</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.89</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5" si="1">F5*G5</f>
+        <v>1.89</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="H6" s="8">
+        <f>F6*G6</f>
+        <v>0.45</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="33">
+        <v>8</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="H9" s="8">
+        <f>F9*G9</f>
+        <v>0.23</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33">
+        <v>9</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="8">
+        <f>F10*G10</f>
+        <v>0.8</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33">
+        <v>10</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33">
+        <v>11</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.18</v>
+      </c>
+      <c r="H12" s="8">
+        <f>F12*G12</f>
+        <v>0.18</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33">
+        <v>12</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="10">
+        <v>6</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*G13</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1.86</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
+        <v>1.86</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H15" s="8">
+        <f>F15*G15</f>
+        <v>0.15</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="33">
+        <v>15</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="12">
+        <v>2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8">
+        <f>F16*G16</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="37">
+        <v>16</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="12">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" ref="H17:H18" si="2">F17*G17</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="37">
+        <v>17</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="12">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="33">
+        <v>18</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>10</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H21" s="8">
+        <f>F21*G21</f>
+        <v>0.15</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>6.52</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="0"/>
+        <v>6.52</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>22</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="19">
+        <v>3</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="8">
+        <f t="shared" ref="H23" si="3">F23*G23</f>
+        <v>3</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q23" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="19">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8">
+        <v>2</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="4">
+        <f>SUM(H3:H25)</f>
+        <v>48.63</v>
+      </c>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="22"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E31" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="17">
+        <f>SUM(H27:H30)+H26</f>
+        <v>48.63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="M9:Q12"/>
+    <mergeCell ref="Q23:U26"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I20" r:id="rId1" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
+    <hyperlink ref="I19" r:id="rId2" location="ht_3637wt_1163" display="http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d - ht_3637wt_1163"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I25" r:id="rId8"/>
+    <hyperlink ref="I14" r:id="rId9"/>
+    <hyperlink ref="I16" r:id="rId10"/>
+    <hyperlink ref="I17" r:id="rId11"/>
+    <hyperlink ref="I18" r:id="rId12"/>
+    <hyperlink ref="I22" r:id="rId13"/>
+    <hyperlink ref="I12" r:id="rId14"/>
+    <hyperlink ref="I9" r:id="rId15"/>
+    <hyperlink ref="I10" r:id="rId16"/>
+    <hyperlink ref="I11" r:id="rId17"/>
+    <hyperlink ref="I23" r:id="rId18"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -921,7 +1972,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>11</v>
@@ -1602,690 +2653,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" activeCellId="1" sqref="H19 H19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7">
-        <v>10</v>
-      </c>
-      <c r="G3" s="8">
-        <f>E3*F3</f>
-        <v>10</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.59</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" ref="G4:G24" si="0">E4*F4</f>
-        <v>0.59</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1.89</v>
-      </c>
-      <c r="G5" s="8">
-        <f t="shared" ref="G5" si="1">E5*F5</f>
-        <v>1.89</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0.45</v>
-      </c>
-      <c r="G6" s="8">
-        <f>E6*F6</f>
-        <v>0.45</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.45</v>
-      </c>
-      <c r="G7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.31</v>
-      </c>
-      <c r="G8" s="8">
-        <f t="shared" si="0"/>
-        <v>0.31</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="G9" s="8">
-        <f>E9*F9</f>
-        <v>0.23</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10">
-        <v>2</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="G10" s="8">
-        <f>E10*F10</f>
-        <v>0.8</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="10">
-        <v>2</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.53</v>
-      </c>
-      <c r="G11" s="8">
-        <f t="shared" si="0"/>
-        <v>1.06</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0.18</v>
-      </c>
-      <c r="G12" s="8">
-        <f>E12*F12</f>
-        <v>0.18</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="10">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1.86</v>
-      </c>
-      <c r="G13" s="8">
-        <f t="shared" si="0"/>
-        <v>1.86</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="12">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G14" s="8">
-        <f>E14*F14</f>
-        <v>0.15</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="12">
-        <v>2</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8">
-        <f>E15*F15</f>
-        <v>2</v>
-      </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="10">
-        <v>6</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G16" s="8">
-        <f>E16*F16</f>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>16</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8">
-        <f t="shared" ref="G17:G18" si="2">E17*F17</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>17</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" s="8">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="8">
-        <v>10</v>
-      </c>
-      <c r="G19" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="8">
-        <v>1.6</v>
-      </c>
-      <c r="G20" s="8">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G21" s="8">
-        <f>E21*F21</f>
-        <v>0.15</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="10">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8">
-        <v>6.52</v>
-      </c>
-      <c r="G22" s="8">
-        <f t="shared" si="0"/>
-        <v>6.52</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>22</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="19">
-        <v>3</v>
-      </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>23</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="0"/>
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="H24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="4">
-        <f>SUM(G3:G24)</f>
-        <v>46.63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="22"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="17">
-        <f>SUM(G26:G29)+G25</f>
-        <v>46.63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1"/>
-    <hyperlink ref="H20" r:id="rId2" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
-    <hyperlink ref="H19" r:id="rId3" location="ht_3637wt_1163" display="http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d - ht_3637wt_1163"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added I2C Pull up resistors
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="11475" windowHeight="5385"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="11475" windowHeight="5325"/>
   </bookViews>
   <sheets>
     <sheet name="Gen2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -371,9 +371,6 @@
     <t>Temp Sensor</t>
   </si>
   <si>
-    <t xml:space="preserve">MeasureBattery </t>
-  </si>
-  <si>
     <t>Photo Cell</t>
   </si>
   <si>
@@ -443,9 +440,6 @@
     <t>Part of battery voltage meter circuit</t>
   </si>
   <si>
-    <t>Part of digital temperature sensor circuit</t>
-  </si>
-  <si>
     <t>Optional - used to connect/disconnect wires quickly without soldering</t>
   </si>
   <si>
@@ -465,6 +459,36 @@
   </si>
   <si>
     <t>Note that posi-lock products come in packages. Try to find cheaper single distributions, or buy with other stromtroopers are share the cost</t>
+  </si>
+  <si>
+    <t>Part of digital temperature sensor circuit, pulls up the OneWire line</t>
+  </si>
+  <si>
+    <t>Temperature Sensor</t>
+  </si>
+  <si>
+    <t>Ri2c</t>
+  </si>
+  <si>
+    <t>Pulls up the LCD I2C SDA and SCL lines</t>
+  </si>
+  <si>
+    <t>I2C Pull Up Resistors - 4.7KOhm, 1/8W</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measure Battery </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detect Gear </t>
   </si>
 </sst>
 </file>
@@ -620,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -656,16 +680,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,6 +691,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -979,14 +1003,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="46.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="40.85546875" customWidth="1"/>
@@ -1036,14 +1061,17 @@
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>109</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1064,11 +1092,11 @@
         <v>58</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="36" t="s">
         <v>115</v>
       </c>
       <c r="B4" s="6">
@@ -1090,18 +1118,18 @@
         <v>0.59</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" ref="H4:H25" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H26" si="0">F4*G4</f>
         <v>0.59</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>110</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="6">
         <v>4</v>
       </c>
@@ -1128,11 +1156,11 @@
         <v>111</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="6">
         <v>5</v>
       </c>
@@ -1159,11 +1187,11 @@
         <v>112</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="6">
         <v>6</v>
       </c>
@@ -1190,11 +1218,11 @@
         <v>113</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="6">
         <v>7</v>
       </c>
@@ -1221,17 +1249,17 @@
         <v>114</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="29">
         <v>8</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="29" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="28" t="s">
@@ -1251,25 +1279,25 @@
         <v>0.23</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="M9" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
+        <v>133</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33">
+      <c r="A10" s="37"/>
+      <c r="B10" s="29">
         <v>9</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="28" t="s">
@@ -1289,23 +1317,23 @@
         <v>0.8</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
+        <v>133</v>
+      </c>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33">
+      <c r="A11" s="37"/>
+      <c r="B11" s="29">
         <v>10</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="29" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="28" t="s">
@@ -1325,23 +1353,23 @@
         <v>1.06</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
+        <v>133</v>
+      </c>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33">
+      <c r="A12" s="37"/>
+      <c r="B12" s="29">
         <v>11</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="29" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="28" t="s">
@@ -1361,23 +1389,23 @@
         <v>0.18</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
+        <v>133</v>
+      </c>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33">
+      <c r="A13" s="37"/>
+      <c r="B13" s="29">
         <v>12</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="31" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1398,12 +1426,12 @@
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>119</v>
+      <c r="A14" s="36" t="s">
+        <v>118</v>
       </c>
       <c r="B14" s="6">
         <v>13</v>
@@ -1428,14 +1456,14 @@
         <v>1.86</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="6">
         <v>14</v>
       </c>
@@ -1460,14 +1488,17 @@
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="33">
+      <c r="A16" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="29">
         <v>15</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1487,20 +1518,20 @@
         <v>2</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="37">
+      <c r="A17" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="33">
         <v>16</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="34" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -1520,18 +1551,18 @@
         <v>1</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="37">
+      <c r="A18" s="36"/>
+      <c r="B18" s="33">
         <v>17</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="34" t="s">
         <v>101</v>
       </c>
       <c r="D18" s="12" t="s">
@@ -1551,20 +1582,20 @@
         <v>1</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="29">
         <v>18</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="31" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="10" t="s">
@@ -1587,226 +1618,255 @@
         <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="29">
+        <v>19</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="12">
+        <v>2</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="8">
+        <f>F20*G20</f>
+        <v>0.3</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="6">
-        <v>19</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="15" t="s">
+      <c r="D21" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="10">
-        <v>1</v>
-      </c>
-      <c r="G20" s="8">
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8">
         <v>1.6</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H21" s="8">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I21" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="J20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="6">
-        <v>20</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="12">
-        <v>1</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="H21" s="8">
-        <f>F21*G21</f>
-        <v>0.15</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6" t="s">
-        <v>142</v>
+      <c r="J21" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
       <c r="B22" s="6">
         <v>21</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="12">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H22" s="8">
+        <f>F22*G22</f>
+        <v>0.15</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="29">
+        <v>22</v>
+      </c>
+      <c r="C23" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="15" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="10">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8">
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
         <v>6.52</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H23" s="8">
         <f t="shared" si="0"/>
         <v>6.52</v>
       </c>
-      <c r="I22" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <v>22</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="I23" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="29">
+        <v>23</v>
+      </c>
+      <c r="C24" s="38" t="s">
         <v>66</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="19">
-        <v>3</v>
-      </c>
-      <c r="G23" s="8">
-        <v>1</v>
-      </c>
-      <c r="H23" s="8">
-        <f t="shared" ref="H23" si="3">F23*G23</f>
-        <v>3</v>
-      </c>
-      <c r="I23" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q23" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
-        <v>23</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="20" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="F24" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" s="8">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" ref="H24" si="3">F24*G24</f>
+        <v>3</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q24" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="29">
+        <v>24</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
+      <c r="G25" s="8">
         <v>2</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H25" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I24" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="I25" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="39"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
-        <v>24</v>
-      </c>
-      <c r="C25" s="29" t="s">
+      <c r="J25" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="29">
+        <v>25</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="20" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
         <v>2.4900000000000002</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H26" s="3">
         <f t="shared" si="0"/>
         <v>2.4900000000000002</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J25" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="4">
-        <f>SUM(H3:H25)</f>
-        <v>48.63</v>
-      </c>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="39"/>
+      <c r="J26" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="6"/>
+      <c r="E27" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4">
+        <f>SUM(H3:H26)</f>
+        <v>48.93</v>
+      </c>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="25"/>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
@@ -1817,52 +1877,59 @@
       <c r="B29" s="6"/>
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="22"/>
-      <c r="H29" s="16"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="22"/>
       <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E31" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="17">
-        <f>SUM(H27:H30)+H26</f>
-        <v>48.63</v>
-      </c>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="M9:Q12"/>
-    <mergeCell ref="Q23:U26"/>
+    <mergeCell ref="Q24:U27"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I20" r:id="rId1" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
+    <hyperlink ref="I21" r:id="rId1" location="ht_2092wt_1163" display="http://www.ebay.com/itm/1-PCS-DS18B20-18B20-Thermometer-Temperature-Sensor-Dalla-/170750980342?pt=LH_DefaultDomain_0&amp;hash=item27c18d30f6 - ht_2092wt_1163"/>
     <hyperlink ref="I19" r:id="rId2" location="ht_3637wt_1163" display="http://www.ebay.com/itm/IIC-I2C-TWI-1602-Serial-Shield-Modle-LCD-Display-For-Arduino-MEGA-2560-UNO-A004-/251052650605?pt=LH_DefaultDomain_0&amp;hash=item3a73e7706d - ht_3637wt_1163"/>
     <hyperlink ref="I4" r:id="rId3"/>
     <hyperlink ref="I5" r:id="rId4"/>
     <hyperlink ref="I6" r:id="rId5"/>
     <hyperlink ref="I7" r:id="rId6"/>
     <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I25" r:id="rId8"/>
+    <hyperlink ref="I26" r:id="rId8"/>
     <hyperlink ref="I14" r:id="rId9"/>
     <hyperlink ref="I16" r:id="rId10"/>
     <hyperlink ref="I17" r:id="rId11"/>
     <hyperlink ref="I18" r:id="rId12"/>
-    <hyperlink ref="I22" r:id="rId13"/>
+    <hyperlink ref="I23" r:id="rId13"/>
     <hyperlink ref="I12" r:id="rId14"/>
     <hyperlink ref="I9" r:id="rId15"/>
     <hyperlink ref="I10" r:id="rId16"/>
     <hyperlink ref="I11" r:id="rId17"/>
-    <hyperlink ref="I23" r:id="rId18"/>
+    <hyperlink ref="I24" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
Fix error with enclosure part #. It should be RP1135C, not RP1085C
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="461">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -1438,6 +1438,12 @@
   </si>
   <si>
     <t>Iduino 328</t>
+  </si>
+  <si>
+    <t>RP1135C</t>
+  </si>
+  <si>
+    <t>RP1135C-ND</t>
   </si>
 </sst>
 </file>
@@ -2034,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,13 +3135,13 @@
         <v>432</v>
       </c>
       <c r="D29" t="s">
-        <v>433</v>
+        <v>459</v>
       </c>
       <c r="E29" t="s">
         <v>166</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>434</v>
+        <v>460</v>
       </c>
       <c r="G29" s="41"/>
       <c r="H29">
@@ -3242,19 +3248,19 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M31"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="42.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Replaced Yellow LED part #
</commit_message>
<xml_diff>
--- a/Project/Stromputer BOM.xlsx
+++ b/Project/Stromputer BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="11475" windowHeight="5325"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="11475" windowHeight="5325" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V3 (Final)" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="462">
   <si>
     <t>Stromputer BOM (Bill Of Materials)</t>
   </si>
@@ -374,9 +374,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/C503B-GCN-CY0C0791/C503B-GCN-CY0C0791-ND/1922940</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en/optoelectronics/leds-discrete/524729?k=67-1117-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?WT.z_header=search_go&amp;lang=en&amp;keywords=C503B-WAN-CCACB151-ND&amp;x=11&amp;y=13&amp;cur=USD</t>
@@ -1444,6 +1441,12 @@
   </si>
   <si>
     <t>RP1135C-ND</t>
+  </si>
+  <si>
+    <t>DIGIKEY: 365-1183-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/OVLFY3C7/365-1183-ND/827119</t>
   </si>
 </sst>
 </file>
@@ -2040,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,57 +2065,57 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C1" s="50" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>454</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>455</v>
       </c>
-      <c r="F1" s="50" t="s">
-        <v>456</v>
-      </c>
       <c r="G1" s="51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="J1" s="50" t="s">
         <v>316</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="K1" s="50" t="s">
         <v>317</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>318</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E2" t="s">
         <v>320</v>
       </c>
-      <c r="D2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="41" t="s">
         <v>322</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>323</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2128,30 +2131,30 @@
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>442</v>
+      </c>
+      <c r="E3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" s="49" t="s">
         <v>325</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>443</v>
-      </c>
-      <c r="E3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F3" s="49" t="s">
+      <c r="G3" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="41" t="s">
-        <v>327</v>
-      </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -2161,36 +2164,36 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" t="s">
         <v>261</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>262</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>263</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G4" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>329</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>330</v>
       </c>
       <c r="J4" s="3">
         <v>0.09</v>
@@ -2200,36 +2203,36 @@
         <v>0.09</v>
       </c>
       <c r="L4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" t="s">
         <v>261</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>262</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>263</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G5" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>332</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>333</v>
       </c>
       <c r="J5" s="3">
         <v>0.09</v>
@@ -2239,36 +2242,36 @@
         <v>0.09</v>
       </c>
       <c r="L5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" t="s">
         <v>261</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>262</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>263</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G6" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>334</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>335</v>
       </c>
       <c r="J6" s="3">
         <v>0.09</v>
@@ -2278,36 +2281,36 @@
         <v>0.09</v>
       </c>
       <c r="L6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" t="s">
         <v>261</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>262</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>263</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G7" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>336</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>337</v>
       </c>
       <c r="J7" s="3">
         <v>0.09</v>
@@ -2317,36 +2320,36 @@
         <v>0.09</v>
       </c>
       <c r="L7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" t="s">
         <v>261</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>262</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>263</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G8" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>338</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>339</v>
       </c>
       <c r="J8" s="3">
         <v>0.09</v>
@@ -2356,36 +2359,36 @@
         <v>0.09</v>
       </c>
       <c r="L8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" t="s">
         <v>261</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>262</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>263</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="G9" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>340</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>341</v>
       </c>
       <c r="J9" s="3">
         <v>0.09</v>
@@ -2395,36 +2398,36 @@
         <v>0.09</v>
       </c>
       <c r="L9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>344</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>345</v>
       </c>
       <c r="J10" s="3">
         <v>0.09</v>
@@ -2434,36 +2437,36 @@
         <v>0.09</v>
       </c>
       <c r="L10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D11" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="G11" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>347</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>348</v>
       </c>
       <c r="J11" s="3">
         <v>0.09</v>
@@ -2473,36 +2476,36 @@
         <v>0.09</v>
       </c>
       <c r="L11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" t="s">
+        <v>341</v>
+      </c>
+      <c r="E12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E12" t="s">
-        <v>166</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="G12" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>350</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>351</v>
       </c>
       <c r="J12" s="3">
         <v>0.09</v>
@@ -2512,30 +2515,30 @@
         <v>0.09</v>
       </c>
       <c r="L12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D13" t="s">
+        <v>351</v>
+      </c>
+      <c r="E13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E13" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="41" t="s">
         <v>353</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>354</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2551,30 +2554,30 @@
         <v>0.09</v>
       </c>
       <c r="L13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" t="s">
         <v>356</v>
       </c>
-      <c r="B14" t="s">
-        <v>237</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>357</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E14" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="41" t="s">
         <v>359</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>360</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2590,30 +2593,30 @@
         <v>1.53</v>
       </c>
       <c r="L14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" t="s">
         <v>356</v>
       </c>
-      <c r="B15" t="s">
-        <v>225</v>
-      </c>
-      <c r="C15" t="s">
-        <v>357</v>
-      </c>
       <c r="D15" t="s">
+        <v>360</v>
+      </c>
+      <c r="E15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="41" t="s">
         <v>362</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>363</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2629,30 +2632,30 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="L15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" t="s">
         <v>356</v>
       </c>
-      <c r="B16" t="s">
-        <v>230</v>
-      </c>
-      <c r="C16" t="s">
-        <v>357</v>
-      </c>
       <c r="D16" t="s">
+        <v>363</v>
+      </c>
+      <c r="E16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E16" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="41" t="s">
         <v>365</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>366</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -2668,30 +2671,30 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="L16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" t="s">
         <v>294</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" t="s">
         <v>295</v>
       </c>
-      <c r="C17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="G17" s="41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2707,30 +2710,30 @@
         <v>0.45</v>
       </c>
       <c r="L17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B18" t="s">
+        <v>370</v>
+      </c>
+      <c r="C18" t="s">
         <v>371</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>372</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E18" t="s">
-        <v>166</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="41" t="s">
         <v>374</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>375</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2746,30 +2749,30 @@
         <v>0.48</v>
       </c>
       <c r="L18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" t="s">
         <v>376</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" t="s">
+        <v>269</v>
+      </c>
+      <c r="E19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G19" s="41" t="s">
         <v>377</v>
-      </c>
-      <c r="C19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" t="s">
-        <v>270</v>
-      </c>
-      <c r="E19" t="s">
-        <v>166</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>378</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2785,27 +2788,27 @@
         <v>0.31</v>
       </c>
       <c r="L19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>378</v>
+      </c>
+      <c r="C20" t="s">
         <v>379</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>380</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E20" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="41" t="s">
         <v>382</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>383</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2821,33 +2824,33 @@
         <v>4.51</v>
       </c>
       <c r="L20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>384</v>
+      </c>
+      <c r="C21" t="s">
         <v>385</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>386</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E21" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="41" t="s">
         <v>388</v>
       </c>
-      <c r="G21" s="41" t="s">
-        <v>389</v>
-      </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J21" s="3">
         <v>19.75</v>
@@ -2857,30 +2860,30 @@
         <v>19.75</v>
       </c>
       <c r="L21" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>390</v>
+      </c>
+      <c r="B22" t="s">
         <v>391</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>392</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>393</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="E22" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="41" t="s">
         <v>395</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>396</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2896,36 +2899,36 @@
         <v>0.21</v>
       </c>
       <c r="L22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B23" t="s">
+        <v>397</v>
+      </c>
+      <c r="C23" t="s">
+        <v>392</v>
+      </c>
+      <c r="D23" t="s">
         <v>398</v>
       </c>
-      <c r="C23" t="s">
-        <v>393</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E23" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="41" t="s">
         <v>400</v>
       </c>
-      <c r="G23" s="41" t="s">
-        <v>401</v>
-      </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J23" s="3">
         <v>0.24</v>
@@ -2935,36 +2938,36 @@
         <v>0.24</v>
       </c>
       <c r="L23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
+        <v>402</v>
+      </c>
+      <c r="C24" t="s">
         <v>403</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>404</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="E24" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="41" t="s">
         <v>406</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>407</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J24" s="3">
         <v>0.55000000000000004</v>
@@ -2974,36 +2977,36 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B25" t="s">
+        <v>408</v>
+      </c>
+      <c r="C25" t="s">
+        <v>392</v>
+      </c>
+      <c r="D25" t="s">
         <v>409</v>
       </c>
-      <c r="C25" t="s">
-        <v>393</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="E25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="41" t="s">
         <v>411</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>412</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J25" s="3">
         <v>0.46</v>
@@ -3013,27 +3016,27 @@
         <v>0.92</v>
       </c>
       <c r="L25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C26" t="s">
+        <v>415</v>
+      </c>
+      <c r="D26" t="s">
         <v>416</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E26" t="s">
-        <v>166</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="41" t="s">
         <v>418</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>419</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -3049,30 +3052,30 @@
         <v>1.68</v>
       </c>
       <c r="L26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B27" s="45">
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" t="s">
+        <v>421</v>
+      </c>
+      <c r="E27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="E27" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="41" t="s">
         <v>423</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>424</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3088,27 +3091,27 @@
         <v>0.59</v>
       </c>
       <c r="L27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>425</v>
+      </c>
+      <c r="C28" t="s">
         <v>426</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>425</v>
+      </c>
+      <c r="E28" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D28" t="s">
-        <v>426</v>
-      </c>
-      <c r="E28" t="s">
-        <v>166</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="41" t="s">
         <v>428</v>
-      </c>
-      <c r="G28" s="41" t="s">
-        <v>429</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3124,24 +3127,24 @@
         <v>1.86</v>
       </c>
       <c r="L28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>430</v>
+      </c>
+      <c r="C29" t="s">
         <v>431</v>
       </c>
-      <c r="C29" t="s">
-        <v>432</v>
-      </c>
       <c r="D29" t="s">
+        <v>458</v>
+      </c>
+      <c r="E29" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="E29" t="s">
-        <v>166</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="G29" s="41"/>
       <c r="H29">
@@ -3155,15 +3158,15 @@
         <v>8.57</v>
       </c>
       <c r="L29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="41"/>
@@ -3181,7 +3184,7 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G31" s="41"/>
       <c r="J31" s="46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K31" s="47">
         <f>SUM(K2:K30)</f>
@@ -3191,37 +3194,37 @@
     <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C36" t="s">
+        <v>445</v>
+      </c>
+      <c r="D36" t="s">
+        <v>447</v>
+      </c>
+      <c r="E36" t="s">
         <v>446</v>
       </c>
-      <c r="D36" t="s">
-        <v>448</v>
-      </c>
-      <c r="E36" t="s">
-        <v>447</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -3234,7 +3237,7 @@
         <v>13.5</v>
       </c>
       <c r="L36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3268,60 +3271,60 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="C1" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="42" t="s">
         <v>310</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="42" t="s">
         <v>312</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="G1" s="42" t="s">
         <v>313</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="H1" s="43" t="s">
         <v>314</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>315</v>
       </c>
       <c r="I1" s="42" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="K1" s="42" t="s">
         <v>316</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="L1" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="M1" s="42" t="s">
         <v>318</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
         <v>320</v>
       </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>321</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="41" t="s">
         <v>322</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>323</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -3337,24 +3340,24 @@
         <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G3" s="44" t="s">
         <v>325</v>
       </c>
-      <c r="B3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" t="s">
-        <v>321</v>
-      </c>
-      <c r="G3" s="44" t="s">
+      <c r="H3" s="41" t="s">
         <v>326</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>327</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3367,39 +3370,39 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
         <v>261</v>
       </c>
-      <c r="B4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>262</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>263</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" t="s">
         <v>264</v>
       </c>
-      <c r="F4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" t="s">
-        <v>265</v>
-      </c>
       <c r="H4" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>329</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>330</v>
       </c>
       <c r="K4" s="3">
         <v>0.09</v>
@@ -3409,39 +3412,39 @@
         <v>0.09</v>
       </c>
       <c r="M4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" t="s">
         <v>261</v>
       </c>
-      <c r="B5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>262</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>263</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
         <v>264</v>
       </c>
-      <c r="F5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G5" t="s">
-        <v>265</v>
-      </c>
       <c r="H5" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>332</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>333</v>
       </c>
       <c r="K5" s="3">
         <v>0.09</v>
@@ -3451,39 +3454,39 @@
         <v>0.09</v>
       </c>
       <c r="M5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
         <v>261</v>
       </c>
-      <c r="B6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>262</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>263</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
         <v>264</v>
       </c>
-      <c r="F6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G6" t="s">
-        <v>265</v>
-      </c>
       <c r="H6" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>334</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>335</v>
       </c>
       <c r="K6" s="3">
         <v>0.09</v>
@@ -3493,39 +3496,39 @@
         <v>0.09</v>
       </c>
       <c r="M6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
         <v>261</v>
       </c>
-      <c r="B7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>262</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>263</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G7" t="s">
         <v>264</v>
       </c>
-      <c r="F7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" t="s">
-        <v>265</v>
-      </c>
       <c r="H7" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>336</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>337</v>
       </c>
       <c r="K7" s="3">
         <v>0.09</v>
@@ -3535,39 +3538,39 @@
         <v>0.09</v>
       </c>
       <c r="M7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
         <v>261</v>
       </c>
-      <c r="B8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>262</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>263</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s">
         <v>264</v>
       </c>
-      <c r="F8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G8" t="s">
-        <v>265</v>
-      </c>
       <c r="H8" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>338</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>339</v>
       </c>
       <c r="K8" s="3">
         <v>0.09</v>
@@ -3577,39 +3580,39 @@
         <v>0.09</v>
       </c>
       <c r="M8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" t="s">
         <v>261</v>
       </c>
-      <c r="B9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>262</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>263</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s">
         <v>264</v>
       </c>
-      <c r="F9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" t="s">
-        <v>265</v>
-      </c>
       <c r="H9" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
         <v>340</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>341</v>
       </c>
       <c r="K9" s="3">
         <v>0.09</v>
@@ -3619,39 +3622,39 @@
         <v>0.09</v>
       </c>
       <c r="M9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E10" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" t="s">
         <v>342</v>
       </c>
-      <c r="F10" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>344</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>345</v>
       </c>
       <c r="K10" s="3">
         <v>0.09</v>
@@ -3661,39 +3664,39 @@
         <v>0.09</v>
       </c>
       <c r="M10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" t="s">
         <v>342</v>
       </c>
-      <c r="F11" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" t="s">
-        <v>343</v>
-      </c>
       <c r="H11" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>347</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>348</v>
       </c>
       <c r="K11" s="3">
         <v>0.09</v>
@@ -3703,39 +3706,39 @@
         <v>0.09</v>
       </c>
       <c r="M11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" t="s">
         <v>342</v>
       </c>
-      <c r="F12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G12" t="s">
-        <v>343</v>
-      </c>
       <c r="H12" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>350</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>351</v>
       </c>
       <c r="K12" s="3">
         <v>0.09</v>
@@ -3745,33 +3748,33 @@
         <v>0.09</v>
       </c>
       <c r="M12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E13" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" t="s">
         <v>352</v>
       </c>
-      <c r="F13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" s="41" t="s">
         <v>353</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>354</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -3787,33 +3790,33 @@
         <v>0.09</v>
       </c>
       <c r="M13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" t="s">
         <v>356</v>
       </c>
-      <c r="B14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>357</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" t="s">
         <v>358</v>
       </c>
-      <c r="F14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" s="41" t="s">
         <v>359</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>360</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -3829,33 +3832,33 @@
         <v>1.53</v>
       </c>
       <c r="M14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" t="s">
         <v>356</v>
       </c>
-      <c r="B15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D15" t="s">
-        <v>357</v>
-      </c>
       <c r="E15" t="s">
+        <v>360</v>
+      </c>
+      <c r="F15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" t="s">
         <v>361</v>
       </c>
-      <c r="F15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" s="41" t="s">
         <v>362</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>363</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -3871,33 +3874,33 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="M15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" t="s">
         <v>356</v>
       </c>
-      <c r="B16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" t="s">
-        <v>357</v>
-      </c>
       <c r="E16" t="s">
+        <v>363</v>
+      </c>
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" t="s">
         <v>364</v>
       </c>
-      <c r="F16" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" s="41" t="s">
         <v>365</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>366</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -3913,33 +3916,33 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="M16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" t="s">
         <v>294</v>
       </c>
-      <c r="B17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" t="s">
         <v>295</v>
       </c>
-      <c r="D17" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" t="s">
         <v>296</v>
       </c>
-      <c r="F17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G17" t="s">
-        <v>297</v>
-      </c>
       <c r="H17" s="41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -3955,33 +3958,33 @@
         <v>0.45</v>
       </c>
       <c r="M17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" t="s">
         <v>369</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>370</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>371</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>372</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" t="s">
         <v>373</v>
       </c>
-      <c r="F18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" s="41" t="s">
         <v>374</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>375</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -3997,33 +4000,33 @@
         <v>0.48</v>
       </c>
       <c r="M18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" t="s">
         <v>376</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" t="s">
         <v>269</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" t="s">
+        <v>270</v>
+      </c>
+      <c r="H19" s="41" t="s">
         <v>377</v>
-      </c>
-      <c r="D19" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" t="s">
-        <v>270</v>
-      </c>
-      <c r="F19" t="s">
-        <v>166</v>
-      </c>
-      <c r="G19" t="s">
-        <v>271</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>378</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -4039,30 +4042,30 @@
         <v>0.31</v>
       </c>
       <c r="M19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>378</v>
+      </c>
+      <c r="B20" t="s">
+        <v>369</v>
+      </c>
+      <c r="D20" t="s">
         <v>379</v>
       </c>
-      <c r="B20" t="s">
-        <v>370</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>380</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" t="s">
         <v>381</v>
       </c>
-      <c r="F20" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" s="41" t="s">
         <v>382</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>383</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -4078,30 +4081,30 @@
         <v>4.51</v>
       </c>
       <c r="M20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>384</v>
+      </c>
+      <c r="B21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
         <v>385</v>
       </c>
-      <c r="B21" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>386</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" t="s">
         <v>387</v>
       </c>
-      <c r="F21" t="s">
-        <v>166</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H21" s="41" t="s">
         <v>388</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>389</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -4114,33 +4117,33 @@
         <v>19.75</v>
       </c>
       <c r="M21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>390</v>
+      </c>
+      <c r="B22" t="s">
+        <v>369</v>
+      </c>
+      <c r="C22" t="s">
         <v>391</v>
       </c>
-      <c r="B22" t="s">
-        <v>370</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>392</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>393</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" t="s">
         <v>394</v>
       </c>
-      <c r="F22" t="s">
-        <v>166</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H22" s="41" t="s">
         <v>395</v>
-      </c>
-      <c r="H22" s="41" t="s">
-        <v>396</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -4153,33 +4156,33 @@
         <v>0.21</v>
       </c>
       <c r="M22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C23" t="s">
+        <v>397</v>
+      </c>
+      <c r="D23" t="s">
+        <v>392</v>
+      </c>
+      <c r="E23" t="s">
         <v>398</v>
       </c>
-      <c r="D23" t="s">
-        <v>393</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" t="s">
         <v>399</v>
       </c>
-      <c r="F23" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" s="41" t="s">
         <v>400</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>401</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -4192,33 +4195,33 @@
         <v>0.24</v>
       </c>
       <c r="M23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C24" t="s">
+        <v>402</v>
+      </c>
+      <c r="D24" t="s">
         <v>403</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>404</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" t="s">
         <v>405</v>
       </c>
-      <c r="F24" t="s">
-        <v>166</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" s="41" t="s">
         <v>406</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>407</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -4231,33 +4234,33 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C25" t="s">
+        <v>408</v>
+      </c>
+      <c r="D25" t="s">
+        <v>392</v>
+      </c>
+      <c r="E25" t="s">
         <v>409</v>
       </c>
-      <c r="D25" t="s">
-        <v>393</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" t="s">
         <v>410</v>
       </c>
-      <c r="F25" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="H25" s="41" t="s">
         <v>411</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>412</v>
       </c>
       <c r="I25">
         <v>2</v>
@@ -4270,30 +4273,30 @@
         <v>0.92</v>
       </c>
       <c r="M25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>413</v>
+      </c>
+      <c r="B26" t="s">
         <v>414</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>415</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>416</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" t="s">
         <v>417</v>
       </c>
-      <c r="F26" t="s">
-        <v>166</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" s="41" t="s">
         <v>418</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>419</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -4309,33 +4312,33 @@
         <v>1.68</v>
       </c>
       <c r="M26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="45">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
+        <v>421</v>
+      </c>
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" t="s">
         <v>422</v>
       </c>
-      <c r="F27" t="s">
-        <v>166</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" s="41" t="s">
         <v>423</v>
-      </c>
-      <c r="H27" s="41" t="s">
-        <v>424</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -4351,30 +4354,30 @@
         <v>0.59</v>
       </c>
       <c r="M27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>425</v>
+      </c>
+      <c r="B28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" t="s">
         <v>426</v>
       </c>
-      <c r="B28" t="s">
-        <v>163</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>425</v>
+      </c>
+      <c r="F28" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" t="s">
         <v>427</v>
       </c>
-      <c r="E28" t="s">
-        <v>426</v>
-      </c>
-      <c r="F28" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="H28" s="41" t="s">
         <v>428</v>
-      </c>
-      <c r="H28" s="41" t="s">
-        <v>429</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -4390,24 +4393,24 @@
         <v>1.86</v>
       </c>
       <c r="M28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>430</v>
+      </c>
+      <c r="D29" t="s">
         <v>431</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>432</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>165</v>
+      </c>
+      <c r="G29" t="s">
         <v>433</v>
-      </c>
-      <c r="F29" t="s">
-        <v>166</v>
-      </c>
-      <c r="G29" t="s">
-        <v>434</v>
       </c>
       <c r="H29" s="41"/>
       <c r="I29">
@@ -4421,15 +4424,15 @@
         <v>8.57</v>
       </c>
       <c r="M29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H30" s="41"/>
       <c r="I30">
@@ -4443,13 +4446,13 @@
         <v>11</v>
       </c>
       <c r="M30" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H31" s="41"/>
       <c r="K31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L31" s="17">
         <f>SUM(L2:L30)</f>
@@ -4458,21 +4461,21 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B35" s="39"/>
       <c r="C35" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D35" s="39"/>
       <c r="E35" s="39"/>
       <c r="F35" s="39"/>
       <c r="G35" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H35" s="39"/>
       <c r="I35" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J35" s="39">
         <v>1</v>
@@ -4484,26 +4487,26 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
       <c r="B36" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="39" t="s">
         <v>162</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>163</v>
       </c>
       <c r="D36" s="39"/>
       <c r="E36" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="F36" s="39" t="s">
+      <c r="G36" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="H36" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="H36" s="39" t="s">
+      <c r="I36" s="40" t="s">
         <v>167</v>
-      </c>
-      <c r="I36" s="40" t="s">
-        <v>168</v>
       </c>
       <c r="J36" s="39">
         <v>1</v>
@@ -4512,16 +4515,16 @@
       <c r="L36" s="39"/>
       <c r="M36" s="3"/>
       <c r="N36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="52"/>
       <c r="B37" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="39" t="s">
         <v>170</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>171</v>
       </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
@@ -4529,7 +4532,7 @@
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
       <c r="I37" s="40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J37" s="39">
         <v>1</v>
@@ -4541,10 +4544,10 @@
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="52"/>
       <c r="B38" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D38" s="39"/>
       <c r="E38" s="39"/>
@@ -4552,7 +4555,7 @@
       <c r="G38" s="39"/>
       <c r="H38" s="39"/>
       <c r="I38" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J38" s="39">
         <v>1</v>
@@ -4561,16 +4564,16 @@
       <c r="L38" s="39"/>
       <c r="M38" s="3"/>
       <c r="N38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
       <c r="B39" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D39" s="39"/>
       <c r="E39" s="39"/>
@@ -4578,7 +4581,7 @@
       <c r="G39" s="39"/>
       <c r="H39" s="39"/>
       <c r="I39" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J39" s="39">
         <v>1</v>
@@ -4587,40 +4590,40 @@
       <c r="L39" s="39"/>
       <c r="M39" s="3"/>
       <c r="N39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
       <c r="B40" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="E40" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="G40" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F40" s="39" t="s">
+      <c r="H40" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G40" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H40" s="39" t="s">
+      <c r="I40" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="I40" s="40" t="s">
+      <c r="J40" s="39">
+        <v>1</v>
+      </c>
+      <c r="K40" s="39" t="s">
         <v>184</v>
-      </c>
-      <c r="J40" s="39">
-        <v>1</v>
-      </c>
-      <c r="K40" s="39" t="s">
-        <v>185</v>
       </c>
       <c r="L40" s="39"/>
       <c r="M40" s="3"/>
@@ -4629,29 +4632,29 @@
       <c r="A41" s="52"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D41" s="39"/>
       <c r="E41" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F41" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F41" s="39" t="s">
+      <c r="G41" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G41" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H41" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I41" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="J41" s="39">
+        <v>1</v>
+      </c>
+      <c r="K41" s="39" t="s">
         <v>186</v>
-      </c>
-      <c r="J41" s="39">
-        <v>1</v>
-      </c>
-      <c r="K41" s="39" t="s">
-        <v>187</v>
       </c>
       <c r="L41" s="39"/>
       <c r="M41" s="3"/>
@@ -4660,29 +4663,29 @@
       <c r="A42" s="52"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D42" s="39"/>
       <c r="E42" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F42" s="39" t="s">
+      <c r="G42" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H42" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G42" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H42" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I42" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="J42" s="39">
+        <v>1</v>
+      </c>
+      <c r="K42" s="39" t="s">
         <v>188</v>
-      </c>
-      <c r="J42" s="39">
-        <v>1</v>
-      </c>
-      <c r="K42" s="39" t="s">
-        <v>189</v>
       </c>
       <c r="L42" s="39"/>
       <c r="M42" s="3"/>
@@ -4691,29 +4694,29 @@
       <c r="A43" s="52"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D43" s="39"/>
       <c r="E43" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F43" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F43" s="39" t="s">
+      <c r="G43" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G43" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H43" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I43" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="J43" s="39">
+        <v>1</v>
+      </c>
+      <c r="K43" s="39" t="s">
         <v>190</v>
-      </c>
-      <c r="J43" s="39">
-        <v>1</v>
-      </c>
-      <c r="K43" s="39" t="s">
-        <v>191</v>
       </c>
       <c r="L43" s="39"/>
       <c r="M43" s="39"/>
@@ -4722,29 +4725,29 @@
       <c r="A44" s="52"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="39"/>
       <c r="E44" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F44" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="39" t="s">
+      <c r="G44" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G44" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H44" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I44" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44" s="39">
+        <v>1</v>
+      </c>
+      <c r="K44" s="39" t="s">
         <v>192</v>
-      </c>
-      <c r="J44" s="39">
-        <v>1</v>
-      </c>
-      <c r="K44" s="39" t="s">
-        <v>193</v>
       </c>
       <c r="L44" s="39"/>
       <c r="M44" s="39"/>
@@ -4753,29 +4756,29 @@
       <c r="A45" s="52"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D45" s="39"/>
       <c r="E45" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F45" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="39" t="s">
+      <c r="G45" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G45" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H45" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I45" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="J45" s="39">
+        <v>1</v>
+      </c>
+      <c r="K45" s="39" t="s">
         <v>194</v>
-      </c>
-      <c r="J45" s="39">
-        <v>1</v>
-      </c>
-      <c r="K45" s="39" t="s">
-        <v>195</v>
       </c>
       <c r="L45" s="39"/>
       <c r="M45" s="39"/>
@@ -4784,29 +4787,29 @@
       <c r="A46" s="52"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D46" s="39"/>
       <c r="E46" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="F46" s="39" t="s">
+      <c r="G46" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H46" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G46" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H46" s="39" t="s">
-        <v>183</v>
-      </c>
       <c r="I46" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="J46" s="39">
+        <v>1</v>
+      </c>
+      <c r="K46" s="39" t="s">
         <v>196</v>
-      </c>
-      <c r="J46" s="39">
-        <v>1</v>
-      </c>
-      <c r="K46" s="39" t="s">
-        <v>197</v>
       </c>
       <c r="L46" s="39"/>
       <c r="M46" s="39"/>
@@ -4814,34 +4817,34 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="52"/>
       <c r="B47" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C47" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F47" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="G47" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D47" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="E47" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F47" s="39" t="s">
+      <c r="H47" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="G47" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H47" s="39" t="s">
+      <c r="I47" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="J47" s="39">
+        <v>1</v>
+      </c>
+      <c r="K47" s="39" t="s">
         <v>201</v>
-      </c>
-      <c r="J47" s="39">
-        <v>1</v>
-      </c>
-      <c r="K47" s="39" t="s">
-        <v>202</v>
       </c>
       <c r="L47" s="39"/>
       <c r="M47" s="39"/>
@@ -4850,29 +4853,29 @@
       <c r="A48" s="52"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D48" s="39"/>
       <c r="E48" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F48" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="I48" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="G48" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H48" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="I48" s="40" t="s">
+      <c r="J48" s="39">
+        <v>1</v>
+      </c>
+      <c r="K48" s="39" t="s">
         <v>204</v>
-      </c>
-      <c r="J48" s="39">
-        <v>1</v>
-      </c>
-      <c r="K48" s="39" t="s">
-        <v>205</v>
       </c>
       <c r="L48" s="39"/>
       <c r="M48" s="39"/>
@@ -4881,29 +4884,29 @@
       <c r="A49" s="52"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D49" s="39"/>
       <c r="E49" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F49" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G49" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H49" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I49" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="J49" s="39">
+        <v>1</v>
+      </c>
+      <c r="K49" s="39" t="s">
         <v>206</v>
-      </c>
-      <c r="J49" s="39">
-        <v>1</v>
-      </c>
-      <c r="K49" s="39" t="s">
-        <v>207</v>
       </c>
       <c r="L49" s="39"/>
       <c r="M49" s="39"/>
@@ -4911,34 +4914,34 @@
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="52"/>
       <c r="B50" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C50" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="G50" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="E50" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F50" s="39" t="s">
+      <c r="H50" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="G50" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H50" s="39" t="s">
+      <c r="I50" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="I50" s="40" t="s">
+      <c r="J50" s="39">
+        <v>1</v>
+      </c>
+      <c r="K50" s="39" t="s">
         <v>211</v>
-      </c>
-      <c r="J50" s="39">
-        <v>1</v>
-      </c>
-      <c r="K50" s="39" t="s">
-        <v>212</v>
       </c>
       <c r="L50" s="39"/>
       <c r="M50" s="39"/>
@@ -4946,28 +4949,28 @@
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="52"/>
       <c r="B51" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D51" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F51" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="E51" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F51" s="39" t="s">
+      <c r="G51" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H51" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="G51" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H51" s="39" t="s">
+      <c r="I51" s="40" t="s">
         <v>215</v>
-      </c>
-      <c r="I51" s="40" t="s">
-        <v>216</v>
       </c>
       <c r="J51" s="39">
         <v>1</v>
@@ -4979,28 +4982,28 @@
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="52"/>
       <c r="B52" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C52" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D52" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="E52" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F52" s="39" t="s">
+      <c r="G52" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H52" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="G52" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H52" s="39" t="s">
+      <c r="I52" s="40" t="s">
         <v>219</v>
-      </c>
-      <c r="I52" s="40" t="s">
-        <v>220</v>
       </c>
       <c r="J52" s="39">
         <v>1</v>
@@ -5012,28 +5015,28 @@
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="52"/>
       <c r="B53" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D53" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="E53" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F53" s="39" t="s">
+      <c r="G53" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="G53" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H53" s="39" t="s">
+      <c r="I53" s="40" t="s">
         <v>223</v>
-      </c>
-      <c r="I53" s="40" t="s">
-        <v>224</v>
       </c>
       <c r="J53" s="39">
         <v>1</v>
@@ -5045,34 +5048,34 @@
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="52"/>
       <c r="B54" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C54" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="G54" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D54" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F54" s="39" t="s">
+      <c r="H54" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="G54" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H54" s="39" t="s">
+      <c r="I54" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="I54" s="40" t="s">
+      <c r="J54" s="39">
+        <v>1</v>
+      </c>
+      <c r="K54" s="39" t="s">
         <v>228</v>
-      </c>
-      <c r="J54" s="39">
-        <v>1</v>
-      </c>
-      <c r="K54" s="39" t="s">
-        <v>229</v>
       </c>
       <c r="L54" s="39"/>
       <c r="M54" s="39"/>
@@ -5080,34 +5083,34 @@
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="52"/>
       <c r="B55" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C55" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F55" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="G55" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F55" s="39" t="s">
+      <c r="H55" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="G55" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H55" s="39" t="s">
+      <c r="I55" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="I55" s="40" t="s">
+      <c r="J55" s="39">
+        <v>1</v>
+      </c>
+      <c r="K55" s="39" t="s">
         <v>233</v>
-      </c>
-      <c r="J55" s="39">
-        <v>1</v>
-      </c>
-      <c r="K55" s="39" t="s">
-        <v>234</v>
       </c>
       <c r="L55" s="39"/>
       <c r="M55" s="39"/>
@@ -5116,29 +5119,29 @@
       <c r="A56" s="52"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D56" s="39"/>
       <c r="E56" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F56" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="G56" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H56" s="39" t="s">
-        <v>232</v>
-      </c>
       <c r="I56" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="J56" s="39">
+        <v>1</v>
+      </c>
+      <c r="K56" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="J56" s="39">
-        <v>1</v>
-      </c>
-      <c r="K56" s="39" t="s">
-        <v>236</v>
       </c>
       <c r="L56" s="39"/>
       <c r="M56" s="39"/>
@@ -5146,34 +5149,34 @@
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="52"/>
       <c r="B57" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C57" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F57" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="G57" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D57" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="E57" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F57" s="39" t="s">
+      <c r="H57" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="G57" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="H57" s="39" t="s">
+      <c r="I57" s="40" t="s">
         <v>239</v>
       </c>
-      <c r="I57" s="40" t="s">
+      <c r="J57" s="39">
+        <v>1</v>
+      </c>
+      <c r="K57" s="39" t="s">
         <v>240</v>
-      </c>
-      <c r="J57" s="39">
-        <v>1</v>
-      </c>
-      <c r="K57" s="39" t="s">
-        <v>241</v>
       </c>
       <c r="L57" s="39"/>
       <c r="M57" s="39"/>
@@ -5181,10 +5184,10 @@
     <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="52"/>
       <c r="B58" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C58" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D58" s="39"/>
       <c r="E58" s="39"/>
@@ -5192,7 +5195,7 @@
       <c r="G58" s="39"/>
       <c r="H58" s="39"/>
       <c r="I58" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J58" s="39">
         <v>4</v>
@@ -5204,26 +5207,26 @@
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="52"/>
       <c r="B59" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C59" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D59" s="39"/>
       <c r="E59" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="F59" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="F59" s="39" t="s">
+      <c r="G59" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H59" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="G59" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H59" s="39" t="s">
+      <c r="I59" s="40" t="s">
         <v>247</v>
-      </c>
-      <c r="I59" s="40" t="s">
-        <v>248</v>
       </c>
       <c r="J59" s="39">
         <v>1</v>
@@ -5234,26 +5237,26 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" s="39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D60" s="39"/>
       <c r="E60" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="F60" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="F60" s="39" t="s">
+      <c r="G60" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H60" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="G60" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H60" s="39" t="s">
+      <c r="I60" s="40" t="s">
         <v>252</v>
-      </c>
-      <c r="I60" s="40" t="s">
-        <v>253</v>
       </c>
       <c r="J60" s="39">
         <v>1</v>
@@ -5262,31 +5265,31 @@
       <c r="L60" s="39"/>
       <c r="M60" s="3"/>
       <c r="N60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D61" s="39"/>
       <c r="E61" s="39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F61" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="G61" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H61" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="G61" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H61" s="39" t="s">
+      <c r="I61" s="40" t="s">
         <v>257</v>
-      </c>
-      <c r="I61" s="40" t="s">
-        <v>258</v>
       </c>
       <c r="J61" s="39">
         <v>1</v>
@@ -5295,15 +5298,15 @@
       <c r="L61" s="39"/>
       <c r="M61" s="3"/>
       <c r="N61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C62" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D62" s="39"/>
       <c r="E62" s="39"/>
@@ -5311,7 +5314,7 @@
       <c r="G62" s="39"/>
       <c r="H62" s="39"/>
       <c r="I62" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J62" s="39">
         <v>1</v>
@@ -5321,34 +5324,34 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="C63" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D63" s="39" t="s">
+      <c r="E63" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="E63" s="39" t="s">
+      <c r="F63" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="F63" s="39" t="s">
+      <c r="G63" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H63" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="G63" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H63" s="39" t="s">
+      <c r="I63" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="I63" s="39" t="s">
+      <c r="J63" s="39">
+        <v>1</v>
+      </c>
+      <c r="K63" s="39" t="s">
         <v>266</v>
-      </c>
-      <c r="J63" s="39">
-        <v>1</v>
-      </c>
-      <c r="K63" s="39" t="s">
-        <v>267</v>
       </c>
       <c r="L63" s="39">
         <v>0.09</v>
@@ -5358,29 +5361,29 @@
         <v>0.09</v>
       </c>
       <c r="N63" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" s="39"/>
       <c r="C64" s="39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D64" s="39"/>
       <c r="E64" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F64" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H64" s="39" t="s">
         <v>270</v>
       </c>
-      <c r="G64" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H64" s="39" t="s">
+      <c r="I64" s="39" t="s">
         <v>271</v>
-      </c>
-      <c r="I64" s="39" t="s">
-        <v>272</v>
       </c>
       <c r="J64" s="39">
         <v>1</v>
@@ -5389,33 +5392,33 @@
       <c r="L64" s="39"/>
       <c r="M64" s="3"/>
       <c r="N64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C65" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="C65" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D65" s="39" t="s">
+      <c r="E65" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="E65" s="39" t="s">
+      <c r="F65" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="F65" s="39" t="s">
+      <c r="G65" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H65" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="I65" s="39" t="s">
         <v>277</v>
-      </c>
-      <c r="G65" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H65" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="I65" s="39" t="s">
-        <v>278</v>
       </c>
       <c r="J65" s="39">
         <v>1</v>
@@ -5424,33 +5427,33 @@
       <c r="L65" s="39"/>
       <c r="M65" s="3"/>
       <c r="N65" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C66" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D66" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="F66" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="E66" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="F66" s="39" t="s">
+      <c r="G66" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H66" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="G66" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H66" s="39" t="s">
+      <c r="I66" s="39" t="s">
         <v>281</v>
-      </c>
-      <c r="I66" s="39" t="s">
-        <v>282</v>
       </c>
       <c r="J66" s="39">
         <v>1</v>
@@ -5459,33 +5462,33 @@
       <c r="L66" s="39"/>
       <c r="M66" s="3"/>
       <c r="N66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C67" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D67" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="F67" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="E67" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="F67" s="39" t="s">
+      <c r="G67" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H67" s="39" t="s">
         <v>284</v>
       </c>
-      <c r="G67" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H67" s="39" t="s">
+      <c r="I67" s="39" t="s">
         <v>285</v>
-      </c>
-      <c r="I67" s="39" t="s">
-        <v>286</v>
       </c>
       <c r="J67" s="39">
         <v>2</v>
@@ -5494,33 +5497,33 @@
       <c r="L67" s="39"/>
       <c r="M67" s="3"/>
       <c r="N67" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="C68" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D68" s="39" t="s">
+      <c r="E68" s="39" t="s">
         <v>288</v>
       </c>
-      <c r="E68" s="39" t="s">
+      <c r="F68" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="F68" s="39" t="s">
+      <c r="G68" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H68" s="39" t="s">
         <v>290</v>
       </c>
-      <c r="G68" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H68" s="39" t="s">
+      <c r="I68" s="39" t="s">
         <v>291</v>
-      </c>
-      <c r="I68" s="39" t="s">
-        <v>292</v>
       </c>
       <c r="J68" s="39">
         <v>1</v>
@@ -5529,33 +5532,33 @@
       <c r="L68" s="39"/>
       <c r="M68" s="3"/>
       <c r="N68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" s="39" t="s">
         <v>294</v>
       </c>
-      <c r="C69" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D69" s="39" t="s">
+      <c r="E69" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F69" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="E69" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" s="39" t="s">
+      <c r="G69" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H69" s="39" t="s">
         <v>296</v>
       </c>
-      <c r="G69" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H69" s="39" t="s">
+      <c r="I69" s="39" t="s">
         <v>297</v>
-      </c>
-      <c r="I69" s="39" t="s">
-        <v>298</v>
       </c>
       <c r="J69" s="39">
         <v>1</v>
@@ -5567,15 +5570,15 @@
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" s="39"/>
       <c r="E70" s="39"/>
@@ -5583,7 +5586,7 @@
       <c r="G70" s="39"/>
       <c r="H70" s="39"/>
       <c r="I70" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J70" s="39">
         <v>2</v>
@@ -5595,25 +5598,25 @@
         <v>0</v>
       </c>
       <c r="N70" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D71" s="39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E71" s="39"/>
       <c r="F71" s="39"/>
       <c r="G71" s="39"/>
       <c r="H71" s="39"/>
       <c r="I71" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J71" s="39">
         <v>2</v>
@@ -5625,25 +5628,25 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C72" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D72" s="39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E72" s="39"/>
       <c r="F72" s="39"/>
       <c r="G72" s="39"/>
       <c r="H72" s="39"/>
       <c r="I72" s="39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J72" s="39">
         <v>1</v>
@@ -5655,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -5671,8 +5674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5727,18 +5730,18 @@
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="29">
         <v>1</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>77</v>
@@ -5758,7 +5761,7 @@
         <v>58</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -5791,7 +5794,7 @@
         <v>109</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5822,7 +5825,7 @@
         <v>110</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -5853,7 +5856,7 @@
         <v>111</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -5884,7 +5887,7 @@
         <v>112</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -5915,7 +5918,7 @@
         <v>113</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5948,10 +5951,10 @@
         <v>118</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M9" s="53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N9" s="53"/>
       <c r="O9" s="53"/>
@@ -5970,23 +5973,23 @@
         <v>85</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>48</v>
+        <v>460</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="8">
-        <v>0.4</v>
+        <v>0.19</v>
       </c>
       <c r="H10" s="8">
         <f>F10*G10</f>
-        <v>0.8</v>
+        <v>0.38</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>119</v>
+        <v>461</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
@@ -6019,10 +6022,10 @@
         <v>1.06</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M11" s="53"/>
       <c r="N11" s="53"/>
@@ -6055,10 +6058,10 @@
         <v>0.18</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M12" s="53"/>
       <c r="N12" s="53"/>
@@ -6092,7 +6095,7 @@
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6122,10 +6125,10 @@
         <v>1.86</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -6154,12 +6157,12 @@
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="29">
         <v>15</v>
@@ -6184,15 +6187,15 @@
         <v>2</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="33">
         <v>16</v>
@@ -6217,10 +6220,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6248,10 +6251,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -6284,7 +6287,7 @@
         <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -6293,10 +6296,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>105</v>
@@ -6313,7 +6316,7 @@
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -6327,7 +6330,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>104</v>
@@ -6346,7 +6349,7 @@
         <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -6375,12 +6378,12 @@
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="29">
         <v>22</v>
@@ -6403,10 +6406,10 @@
         <v>6.52</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -6435,10 +6438,10 @@
         <v>67</v>
       </c>
       <c r="J24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q24" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R24" s="53"/>
       <c r="S24" s="53"/>
@@ -6451,11 +6454,11 @@
         <v>24</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F25" s="19">
         <v>1</v>
@@ -6468,10 +6471,10 @@
         <v>9</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q25" s="53"/>
       <c r="R25" s="53"/>
@@ -6505,7 +6508,7 @@
         <v>94</v>
       </c>
       <c r="J26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q26" s="53"/>
       <c r="R26" s="53"/>
@@ -6515,13 +6518,13 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="4">
         <f>SUM(H3:H26)</f>
-        <v>61.93</v>
+        <v>61.51</v>
       </c>
       <c r="Q27" s="53"/>
       <c r="R27" s="53"/>
@@ -6593,9 +6596,9 @@
     <hyperlink ref="I23" r:id="rId13"/>
     <hyperlink ref="I12" r:id="rId14"/>
     <hyperlink ref="I9" r:id="rId15"/>
-    <hyperlink ref="I10" r:id="rId16"/>
-    <hyperlink ref="I11" r:id="rId17"/>
-    <hyperlink ref="I24" r:id="rId18"/>
+    <hyperlink ref="I11" r:id="rId16"/>
+    <hyperlink ref="I24" r:id="rId17"/>
+    <hyperlink ref="I10" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -6607,7 +6610,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>